<commit_message>
add moist rod model
</commit_message>
<xml_diff>
--- a/Lab/Transient results/parameter values.xlsx
+++ b/Lab/Transient results/parameter values.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Experiment</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>1113 &lt; c &lt; 1188</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>power loss = 0 +- 0.8 W</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -161,12 +170,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -229,9 +254,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:N7" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:N7"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:P7" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:P7"/>
+  <tableColumns count="16">
     <tableColumn id="1" name="Experiment"/>
     <tableColumn id="2" name="k"/>
     <tableColumn id="3" name="deltak"/>
@@ -239,13 +264,15 @@
     <tableColumn id="5" name="deltakc"/>
     <tableColumn id="6" name="eps"/>
     <tableColumn id="7" name="deltaeps"/>
-    <tableColumn id="8" name="kcend" dataDxfId="4"/>
-    <tableColumn id="9" name="deltakcend" dataDxfId="3"/>
-    <tableColumn id="10" name="epsend" dataDxfId="2"/>
-    <tableColumn id="11" name="deltaepsend" dataDxfId="1"/>
+    <tableColumn id="8" name="kcend" dataDxfId="6"/>
+    <tableColumn id="9" name="deltakcend" dataDxfId="5"/>
+    <tableColumn id="10" name="epsend" dataDxfId="4"/>
+    <tableColumn id="11" name="deltaepsend" dataDxfId="3"/>
     <tableColumn id="12" name="c"/>
     <tableColumn id="13" name="deltac"/>
-    <tableColumn id="14" name="Uncertainty" dataDxfId="0"/>
+    <tableColumn id="14" name="Uncertainty" dataDxfId="2"/>
+    <tableColumn id="15" name="Column1" dataDxfId="1"/>
+    <tableColumn id="16" name="Column2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -514,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +565,7 @@
     <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -581,8 +608,14 @@
       <c r="N1" t="s">
         <v>19</v>
       </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -626,8 +659,9 @@
         <v>5.62</v>
       </c>
       <c r="O2" s="3"/>
+      <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -663,8 +697,9 @@
         <v>2.66</v>
       </c>
       <c r="O3" s="3"/>
+      <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -700,8 +735,9 @@
         <v>2.4</v>
       </c>
       <c r="O4" s="3"/>
+      <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -737,19 +773,49 @@
         <v>4.1399999999999997</v>
       </c>
       <c r="O5" s="3"/>
+      <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
+      </c>
+      <c r="B6">
+        <v>191</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+      <c r="D6">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.6</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="3"/>
+      <c r="L6">
+        <v>1381</v>
+      </c>
+      <c r="M6">
+        <v>600</v>
+      </c>
+      <c r="N6" s="2">
+        <v>3.45</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -785,8 +851,9 @@
         <v>2</v>
       </c>
       <c r="O7" s="3"/>
+      <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>20</v>
       </c>

</xml_diff>